<commit_message>
API design updated with the requirement
</commit_message>
<xml_diff>
--- a/API-Design_Md Aamir Hussain.xlsx
+++ b/API-Design_Md Aamir Hussain.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="59">
   <si>
     <t>NO</t>
   </si>
@@ -52,17 +52,6 @@
   </si>
   <si>
     <t>content-type : application/json</t>
-  </si>
-  <si>
-    <t>[
-{
-    "bookId": "1",
-    "bookName": "Two States"
-}
-]</t>
-  </si>
-  <si>
-    <t>Guest, Reader and Author can search books</t>
   </si>
   <si>
     <t>Authorization : Bearer eyJhbGciOiJIUzI</t>
@@ -84,9 +73,6 @@
     "userName": "abcd",
     "password": "Abcd@1234"
 }</t>
-  </si>
-  <si>
-    <t>Guest can get login</t>
   </si>
   <si>
     <t>/{book-id}/subscribe</t>
@@ -272,6 +258,32 @@
   </si>
   <si>
     <t>/readers/{emailId}/books/{subscription-id}/cancel-subscription within 24 hrs</t>
+  </si>
+  <si>
+    <t>Path variable- category&amp;title&amp;author&amp;price&amp;publisher</t>
+  </si>
+  <si>
+    <t>[
+{
+ logo: image
+ title: Spiderman is back
+category: comic
+price: 24
+author: {book auther name}
+publisher: Moon publisher
+published date: 22/04/2022 
+}
+]</t>
+  </si>
+  <si>
+    <t>Guest, Reader and Author can search books
+Authentication not required.</t>
+  </si>
+  <si>
+    <t>Guest can get login as role READER/AUTHER</t>
+  </si>
+  <si>
+    <t>Auther can edit the book.</t>
   </si>
 </sst>
 </file>
@@ -492,21 +504,18 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -517,6 +526,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -732,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
-      <selection activeCell="B211" sqref="B211:B236"/>
+    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="A211" sqref="A211:A236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -817,14 +829,14 @@
         <v>10</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="23">
+      <c r="F3" s="27">
         <v>200</v>
       </c>
-      <c r="G3" s="17" t="s">
-        <v>11</v>
+      <c r="G3" s="20" t="s">
+        <v>55</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="38.25" customHeight="1">
@@ -832,7 +844,7 @@
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
       <c r="D4" s="6" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="18"/>
@@ -959,7 +971,7 @@
         <v>401</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H16" s="18"/>
     </row>
@@ -1001,26 +1013,26 @@
     </row>
     <row r="20" spans="1:8" ht="14.25" customHeight="1">
       <c r="A20" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" s="20">
+      <c r="E20" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="17">
         <v>201</v>
       </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17" t="s">
-        <v>55</v>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="14.25" customHeight="1">
@@ -1079,11 +1091,11 @@
       <c r="C26" s="18"/>
       <c r="D26" s="7"/>
       <c r="E26" s="12"/>
-      <c r="F26" s="20">
+      <c r="F26" s="17">
         <v>401</v>
       </c>
       <c r="G26" s="13"/>
-      <c r="H26" s="17"/>
+      <c r="H26" s="20"/>
     </row>
     <row r="27" spans="1:8" ht="14.25" customHeight="1">
       <c r="A27" s="18"/>
@@ -1107,35 +1119,33 @@
     </row>
     <row r="29" spans="1:8" ht="14.25" customHeight="1">
       <c r="A29" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B29" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="22" t="s">
         <v>15</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>17</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="20">
+      <c r="E29" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="17">
         <v>200</v>
       </c>
-      <c r="G29" s="20"/>
-      <c r="H29" s="17" t="s">
-        <v>19</v>
+      <c r="G29" s="17"/>
+      <c r="H29" s="20" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="14.25" customHeight="1">
       <c r="A30" s="18"/>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
-      <c r="D30" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="D30" s="6"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
@@ -1247,11 +1257,11 @@
       <c r="C41" s="18"/>
       <c r="D41" s="7"/>
       <c r="E41" s="18"/>
-      <c r="F41" s="20">
+      <c r="F41" s="17">
         <v>401</v>
       </c>
       <c r="G41" s="13"/>
-      <c r="H41" s="17"/>
+      <c r="H41" s="20"/>
     </row>
     <row r="42" spans="1:8" ht="14.25" customHeight="1">
       <c r="A42" s="18"/>
@@ -1275,28 +1285,28 @@
     </row>
     <row r="44" spans="1:8" ht="14.25" customHeight="1">
       <c r="A44" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F44" s="20">
+      <c r="E44" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="17">
         <v>200</v>
       </c>
-      <c r="G44" s="20" t="s">
-        <v>22</v>
+      <c r="G44" s="17" t="s">
+        <v>19</v>
       </c>
       <c r="H44" s="22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="14.25" customHeight="1">
@@ -1304,7 +1314,7 @@
       <c r="B45" s="18"/>
       <c r="C45" s="18"/>
       <c r="D45" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
@@ -1377,11 +1387,11 @@
       <c r="C52" s="18"/>
       <c r="D52" s="7"/>
       <c r="E52" s="18"/>
-      <c r="F52" s="20">
+      <c r="F52" s="17">
         <v>401</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H52" s="18"/>
     </row>
@@ -1393,44 +1403,44 @@
       <c r="E53" s="18"/>
       <c r="F53" s="18"/>
       <c r="G53" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H53" s="18"/>
     </row>
     <row r="54" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A54" s="24"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24"/>
+      <c r="A54" s="23"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="23"/>
       <c r="D54" s="7"/>
-      <c r="E54" s="24"/>
+      <c r="E54" s="23"/>
       <c r="F54" s="19"/>
       <c r="G54" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H54" s="19"/>
     </row>
     <row r="55" spans="1:8" ht="14.25" customHeight="1">
       <c r="A55" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B55" s="22" t="s">
         <v>8</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="17"/>
-      <c r="F55" s="20">
+      <c r="E55" s="20"/>
+      <c r="F55" s="17">
         <v>200</v>
       </c>
-      <c r="G55" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="H55" s="17" t="s">
-        <v>29</v>
+      <c r="G55" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H55" s="20" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="14.25" customHeight="1">
@@ -1438,7 +1448,7 @@
       <c r="B56" s="18"/>
       <c r="C56" s="18"/>
       <c r="D56" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E56" s="18"/>
       <c r="F56" s="18"/>
@@ -1511,13 +1521,13 @@
       <c r="C63" s="18"/>
       <c r="D63" s="7"/>
       <c r="E63" s="18"/>
-      <c r="F63" s="20">
+      <c r="F63" s="17">
         <v>401</v>
       </c>
       <c r="G63" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H63" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="H63" s="20"/>
     </row>
     <row r="64" spans="1:8" ht="14.25" customHeight="1">
       <c r="A64" s="18"/>
@@ -1527,7 +1537,7 @@
       <c r="E64" s="18"/>
       <c r="F64" s="18"/>
       <c r="G64" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H64" s="18"/>
     </row>
@@ -1539,7 +1549,7 @@
       <c r="E65" s="18"/>
       <c r="F65" s="19"/>
       <c r="G65" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H65" s="19"/>
     </row>
@@ -1549,13 +1559,13 @@
       <c r="C66" s="18"/>
       <c r="D66" s="7"/>
       <c r="E66" s="18"/>
-      <c r="F66" s="20">
+      <c r="F66" s="17">
         <v>404</v>
       </c>
       <c r="G66" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H66" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="H66" s="20"/>
     </row>
     <row r="67" spans="1:8" ht="14.25" customHeight="1">
       <c r="A67" s="18"/>
@@ -1565,7 +1575,7 @@
       <c r="E67" s="18"/>
       <c r="F67" s="18"/>
       <c r="G67" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H67" s="18"/>
     </row>
@@ -1577,34 +1587,34 @@
       <c r="E68" s="19"/>
       <c r="F68" s="19"/>
       <c r="G68" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H68" s="19"/>
     </row>
     <row r="69" spans="1:8" ht="14.25" customHeight="1">
       <c r="A69" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B69" s="22" t="s">
         <v>8</v>
       </c>
       <c r="C69" s="22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E69" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F69" s="20">
+      <c r="E69" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F69" s="17">
         <v>200</v>
       </c>
-      <c r="G69" s="17" t="s">
-        <v>33</v>
+      <c r="G69" s="20" t="s">
+        <v>30</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="14.25" customHeight="1">
@@ -1612,7 +1622,7 @@
       <c r="B70" s="18"/>
       <c r="C70" s="18"/>
       <c r="D70" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E70" s="18"/>
       <c r="F70" s="18"/>
@@ -1735,13 +1745,13 @@
       <c r="C82" s="18"/>
       <c r="D82" s="7"/>
       <c r="E82" s="18"/>
-      <c r="F82" s="20">
+      <c r="F82" s="17">
         <v>401</v>
       </c>
       <c r="G82" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H82" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="H82" s="20"/>
     </row>
     <row r="83" spans="1:8" ht="14.25" customHeight="1">
       <c r="A83" s="18"/>
@@ -1751,7 +1761,7 @@
       <c r="E83" s="18"/>
       <c r="F83" s="18"/>
       <c r="G83" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H83" s="18"/>
     </row>
@@ -1763,7 +1773,7 @@
       <c r="E84" s="18"/>
       <c r="F84" s="19"/>
       <c r="G84" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H84" s="19"/>
     </row>
@@ -1773,13 +1783,13 @@
       <c r="C85" s="18"/>
       <c r="D85" s="7"/>
       <c r="E85" s="18"/>
-      <c r="F85" s="20">
+      <c r="F85" s="17">
         <v>404</v>
       </c>
       <c r="G85" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H85" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="H85" s="20"/>
     </row>
     <row r="86" spans="1:8" ht="14.25" customHeight="1">
       <c r="A86" s="18"/>
@@ -1789,7 +1799,7 @@
       <c r="E86" s="18"/>
       <c r="F86" s="18"/>
       <c r="G86" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H86" s="18"/>
     </row>
@@ -1801,32 +1811,32 @@
       <c r="E87" s="19"/>
       <c r="F87" s="19"/>
       <c r="G87" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H87" s="19"/>
     </row>
     <row r="88" spans="1:8" ht="14.25" customHeight="1">
       <c r="A88" s="21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B88" s="22" t="s">
         <v>8</v>
       </c>
       <c r="C88" s="22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E88" s="17"/>
-      <c r="F88" s="20">
+      <c r="E88" s="20"/>
+      <c r="F88" s="17">
         <v>200</v>
       </c>
-      <c r="G88" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="H88" s="17" t="s">
-        <v>37</v>
+      <c r="G88" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H88" s="20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="14.25" customHeight="1">
@@ -1834,7 +1844,7 @@
       <c r="B89" s="18"/>
       <c r="C89" s="18"/>
       <c r="D89" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E89" s="18"/>
       <c r="F89" s="18"/>
@@ -2057,13 +2067,13 @@
       <c r="C111" s="18"/>
       <c r="D111" s="7"/>
       <c r="E111" s="18"/>
-      <c r="F111" s="20">
+      <c r="F111" s="17">
         <v>401</v>
       </c>
       <c r="G111" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H111" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="H111" s="20"/>
     </row>
     <row r="112" spans="1:8" ht="14.25" customHeight="1">
       <c r="A112" s="18"/>
@@ -2073,7 +2083,7 @@
       <c r="E112" s="18"/>
       <c r="F112" s="18"/>
       <c r="G112" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H112" s="18"/>
     </row>
@@ -2085,40 +2095,40 @@
       <c r="E113" s="19"/>
       <c r="F113" s="19"/>
       <c r="G113" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H113" s="19"/>
     </row>
     <row r="114" spans="1:8" ht="14.25" customHeight="1">
       <c r="A114" s="21">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B114" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C114" s="25" t="s">
-        <v>56</v>
+        <v>13</v>
+      </c>
+      <c r="C114" s="24" t="s">
+        <v>53</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E114" s="5"/>
-      <c r="F114" s="20">
+      <c r="F114" s="17">
         <v>201</v>
       </c>
-      <c r="G114" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="H114" s="17" t="s">
-        <v>39</v>
+      <c r="G114" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H114" s="20" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="14.25" customHeight="1">
       <c r="A115" s="18"/>
       <c r="B115" s="18"/>
-      <c r="C115" s="26"/>
+      <c r="C115" s="25"/>
       <c r="D115" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E115" s="6"/>
       <c r="F115" s="18"/>
@@ -2128,7 +2138,7 @@
     <row r="116" spans="1:8" ht="14.25" customHeight="1">
       <c r="A116" s="18"/>
       <c r="B116" s="18"/>
-      <c r="C116" s="26"/>
+      <c r="C116" s="25"/>
       <c r="D116" s="7"/>
       <c r="E116" s="6"/>
       <c r="F116" s="18"/>
@@ -2138,7 +2148,7 @@
     <row r="117" spans="1:8" ht="14.25" customHeight="1">
       <c r="A117" s="18"/>
       <c r="B117" s="18"/>
-      <c r="C117" s="26"/>
+      <c r="C117" s="25"/>
       <c r="D117" s="7"/>
       <c r="E117" s="6"/>
       <c r="F117" s="18"/>
@@ -2148,7 +2158,7 @@
     <row r="118" spans="1:8" ht="14.25" customHeight="1">
       <c r="A118" s="18"/>
       <c r="B118" s="18"/>
-      <c r="C118" s="26"/>
+      <c r="C118" s="25"/>
       <c r="D118" s="7"/>
       <c r="E118" s="6"/>
       <c r="F118" s="18"/>
@@ -2158,7 +2168,7 @@
     <row r="119" spans="1:8" ht="14.25" customHeight="1">
       <c r="A119" s="18"/>
       <c r="B119" s="18"/>
-      <c r="C119" s="26"/>
+      <c r="C119" s="25"/>
       <c r="D119" s="7"/>
       <c r="E119" s="6"/>
       <c r="F119" s="18"/>
@@ -2168,7 +2178,7 @@
     <row r="120" spans="1:8" ht="14.25" customHeight="1">
       <c r="A120" s="18"/>
       <c r="B120" s="18"/>
-      <c r="C120" s="26"/>
+      <c r="C120" s="25"/>
       <c r="D120" s="7"/>
       <c r="E120" s="6"/>
       <c r="F120" s="18"/>
@@ -2178,7 +2188,7 @@
     <row r="121" spans="1:8" ht="14.25" customHeight="1">
       <c r="A121" s="18"/>
       <c r="B121" s="18"/>
-      <c r="C121" s="26"/>
+      <c r="C121" s="25"/>
       <c r="D121" s="7"/>
       <c r="E121" s="6"/>
       <c r="F121" s="18"/>
@@ -2188,7 +2198,7 @@
     <row r="122" spans="1:8" ht="14.25" customHeight="1">
       <c r="A122" s="18"/>
       <c r="B122" s="18"/>
-      <c r="C122" s="26"/>
+      <c r="C122" s="25"/>
       <c r="D122" s="7"/>
       <c r="E122" s="6"/>
       <c r="F122" s="18"/>
@@ -2198,7 +2208,7 @@
     <row r="123" spans="1:8" ht="14.25" customHeight="1">
       <c r="A123" s="18"/>
       <c r="B123" s="18"/>
-      <c r="C123" s="26"/>
+      <c r="C123" s="25"/>
       <c r="D123" s="7"/>
       <c r="E123" s="6"/>
       <c r="F123" s="18"/>
@@ -2208,7 +2218,7 @@
     <row r="124" spans="1:8" ht="14.25" customHeight="1">
       <c r="A124" s="18"/>
       <c r="B124" s="18"/>
-      <c r="C124" s="26"/>
+      <c r="C124" s="25"/>
       <c r="D124" s="7"/>
       <c r="E124" s="6"/>
       <c r="F124" s="18"/>
@@ -2218,7 +2228,7 @@
     <row r="125" spans="1:8" ht="14.25" customHeight="1">
       <c r="A125" s="18"/>
       <c r="B125" s="18"/>
-      <c r="C125" s="26"/>
+      <c r="C125" s="25"/>
       <c r="D125" s="7"/>
       <c r="E125" s="6"/>
       <c r="F125" s="18"/>
@@ -2228,7 +2238,7 @@
     <row r="126" spans="1:8" ht="14.25" customHeight="1">
       <c r="A126" s="18"/>
       <c r="B126" s="18"/>
-      <c r="C126" s="26"/>
+      <c r="C126" s="25"/>
       <c r="D126" s="7"/>
       <c r="E126" s="6"/>
       <c r="F126" s="18"/>
@@ -2238,7 +2248,7 @@
     <row r="127" spans="1:8" ht="14.25" customHeight="1">
       <c r="A127" s="18"/>
       <c r="B127" s="18"/>
-      <c r="C127" s="26"/>
+      <c r="C127" s="25"/>
       <c r="D127" s="7"/>
       <c r="E127" s="6"/>
       <c r="F127" s="18"/>
@@ -2248,7 +2258,7 @@
     <row r="128" spans="1:8" ht="14.25" customHeight="1">
       <c r="A128" s="18"/>
       <c r="B128" s="18"/>
-      <c r="C128" s="26"/>
+      <c r="C128" s="25"/>
       <c r="D128" s="7"/>
       <c r="E128" s="6"/>
       <c r="F128" s="18"/>
@@ -2258,7 +2268,7 @@
     <row r="129" spans="1:8" ht="14.25" customHeight="1" thickBot="1">
       <c r="A129" s="18"/>
       <c r="B129" s="18"/>
-      <c r="C129" s="26"/>
+      <c r="C129" s="25"/>
       <c r="D129" s="7"/>
       <c r="E129" s="6"/>
       <c r="F129" s="19"/>
@@ -2268,65 +2278,65 @@
     <row r="130" spans="1:8" ht="14.25" customHeight="1">
       <c r="A130" s="18"/>
       <c r="B130" s="18"/>
-      <c r="C130" s="26"/>
+      <c r="C130" s="25"/>
       <c r="D130" s="7"/>
       <c r="E130" s="6"/>
-      <c r="F130" s="20">
+      <c r="F130" s="17">
         <v>401</v>
       </c>
       <c r="G130" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H130" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="H130" s="20"/>
     </row>
     <row r="131" spans="1:8" ht="14.25" customHeight="1">
       <c r="A131" s="18"/>
       <c r="B131" s="18"/>
-      <c r="C131" s="26"/>
+      <c r="C131" s="25"/>
       <c r="D131" s="7"/>
       <c r="E131" s="7"/>
       <c r="F131" s="18"/>
       <c r="G131" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H131" s="18"/>
     </row>
     <row r="132" spans="1:8" ht="14.25" customHeight="1" thickBot="1">
       <c r="A132" s="19"/>
       <c r="B132" s="19"/>
-      <c r="C132" s="27"/>
+      <c r="C132" s="26"/>
       <c r="D132" s="9"/>
       <c r="E132" s="9"/>
       <c r="F132" s="19"/>
       <c r="G132" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H132" s="19"/>
     </row>
     <row r="133" spans="1:8" ht="14.25" customHeight="1">
       <c r="A133" s="21">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B133" s="22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C133" s="22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D133" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E133" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="F133" s="20">
+      <c r="E133" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F133" s="17">
         <v>200</v>
       </c>
-      <c r="G133" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="H133" s="17" t="s">
-        <v>43</v>
+      <c r="G133" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H133" s="20" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="14.25" customHeight="1">
@@ -2334,7 +2344,7 @@
       <c r="B134" s="18"/>
       <c r="C134" s="18"/>
       <c r="D134" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E134" s="18"/>
       <c r="F134" s="18"/>
@@ -2527,13 +2537,13 @@
       <c r="C153" s="18"/>
       <c r="D153" s="7"/>
       <c r="E153" s="18"/>
-      <c r="F153" s="20">
+      <c r="F153" s="17">
         <v>401</v>
       </c>
       <c r="G153" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H153" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="H153" s="20"/>
     </row>
     <row r="154" spans="1:8" ht="14.25" customHeight="1">
       <c r="A154" s="18"/>
@@ -2543,7 +2553,7 @@
       <c r="E154" s="18"/>
       <c r="F154" s="18"/>
       <c r="G154" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H154" s="18"/>
     </row>
@@ -2555,7 +2565,7 @@
       <c r="E155" s="18"/>
       <c r="F155" s="19"/>
       <c r="G155" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H155" s="19"/>
     </row>
@@ -2565,13 +2575,13 @@
       <c r="C156" s="18"/>
       <c r="D156" s="7"/>
       <c r="E156" s="18"/>
-      <c r="F156" s="20">
+      <c r="F156" s="17">
         <v>400</v>
       </c>
       <c r="G156" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H156" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="H156" s="20"/>
     </row>
     <row r="157" spans="1:8" ht="14.25" customHeight="1">
       <c r="A157" s="18"/>
@@ -2581,7 +2591,7 @@
       <c r="E157" s="18"/>
       <c r="F157" s="18"/>
       <c r="G157" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H157" s="18"/>
     </row>
@@ -2593,40 +2603,42 @@
       <c r="E158" s="19"/>
       <c r="F158" s="19"/>
       <c r="G158" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H158" s="19"/>
     </row>
     <row r="159" spans="1:8" ht="14.25" customHeight="1">
       <c r="A159" s="21">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B159" s="22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C159" s="22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D159" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E159" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F159" s="20">
+      <c r="E159" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F159" s="17">
         <v>200</v>
       </c>
-      <c r="G159" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="H159" s="17"/>
+      <c r="G159" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H159" s="20" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="160" spans="1:8" ht="14.25" customHeight="1">
       <c r="A160" s="18"/>
       <c r="B160" s="18"/>
       <c r="C160" s="18"/>
       <c r="D160" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E160" s="18"/>
       <c r="F160" s="18"/>
@@ -2849,13 +2861,13 @@
       <c r="C182" s="18"/>
       <c r="D182" s="7"/>
       <c r="E182" s="18"/>
-      <c r="F182" s="20">
+      <c r="F182" s="17">
         <v>401</v>
       </c>
       <c r="G182" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H182" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="H182" s="20"/>
     </row>
     <row r="183" spans="1:8" ht="14.25" customHeight="1">
       <c r="A183" s="18"/>
@@ -2865,7 +2877,7 @@
       <c r="E183" s="18"/>
       <c r="F183" s="18"/>
       <c r="G183" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H183" s="18"/>
     </row>
@@ -2877,32 +2889,32 @@
       <c r="E184" s="19"/>
       <c r="F184" s="19"/>
       <c r="G184" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H184" s="19"/>
     </row>
     <row r="185" spans="1:8" ht="14.25" customHeight="1">
       <c r="A185" s="21">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B185" s="22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C185" s="22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D185" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E185" s="17"/>
-      <c r="F185" s="20">
+      <c r="E185" s="20"/>
+      <c r="F185" s="17">
         <v>200</v>
       </c>
-      <c r="G185" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="H185" s="17" t="s">
-        <v>50</v>
+      <c r="G185" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H185" s="20" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="186" spans="1:8" ht="14.25" customHeight="1">
@@ -2910,7 +2922,7 @@
       <c r="B186" s="18"/>
       <c r="C186" s="18"/>
       <c r="D186" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E186" s="18"/>
       <c r="F186" s="18"/>
@@ -3133,13 +3145,13 @@
       <c r="C208" s="18"/>
       <c r="D208" s="7"/>
       <c r="E208" s="18"/>
-      <c r="F208" s="20">
+      <c r="F208" s="17">
         <v>401</v>
       </c>
       <c r="G208" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H208" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="H208" s="20"/>
     </row>
     <row r="209" spans="1:8" ht="14.25" customHeight="1">
       <c r="A209" s="18"/>
@@ -3149,7 +3161,7 @@
       <c r="E209" s="18"/>
       <c r="F209" s="18"/>
       <c r="G209" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H209" s="18"/>
     </row>
@@ -3161,32 +3173,32 @@
       <c r="E210" s="19"/>
       <c r="F210" s="19"/>
       <c r="G210" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H210" s="19"/>
     </row>
     <row r="211" spans="1:8" ht="14.25" customHeight="1">
       <c r="A211" s="21">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B211" s="22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C211" s="22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D211" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E211" s="17"/>
-      <c r="F211" s="20">
+      <c r="E211" s="20"/>
+      <c r="F211" s="17">
         <v>200</v>
       </c>
-      <c r="G211" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="H211" s="17" t="s">
-        <v>53</v>
+      <c r="G211" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H211" s="20" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="212" spans="1:8" ht="14.25" customHeight="1">
@@ -3194,7 +3206,7 @@
       <c r="B212" s="18"/>
       <c r="C212" s="18"/>
       <c r="D212" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E212" s="18"/>
       <c r="F212" s="18"/>
@@ -3417,13 +3429,13 @@
       <c r="C234" s="18"/>
       <c r="D234" s="7"/>
       <c r="E234" s="18"/>
-      <c r="F234" s="20">
+      <c r="F234" s="17">
         <v>401</v>
       </c>
       <c r="G234" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H234" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="H234" s="20"/>
     </row>
     <row r="235" spans="1:8" ht="14.25" customHeight="1">
       <c r="A235" s="18"/>
@@ -3433,7 +3445,7 @@
       <c r="E235" s="18"/>
       <c r="F235" s="18"/>
       <c r="G235" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H235" s="18"/>
     </row>
@@ -3445,7 +3457,7 @@
       <c r="E236" s="19"/>
       <c r="F236" s="19"/>
       <c r="G236" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H236" s="19"/>
     </row>
@@ -4215,18 +4227,78 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="108">
-    <mergeCell ref="F159:F181"/>
-    <mergeCell ref="G159:G181"/>
-    <mergeCell ref="H159:H181"/>
-    <mergeCell ref="F182:F184"/>
-    <mergeCell ref="H182:H184"/>
-    <mergeCell ref="F85:F87"/>
-    <mergeCell ref="F88:F110"/>
-    <mergeCell ref="F114:F129"/>
-    <mergeCell ref="G114:G129"/>
-    <mergeCell ref="F130:F132"/>
-    <mergeCell ref="F133:F152"/>
-    <mergeCell ref="G133:G152"/>
+    <mergeCell ref="A3:A19"/>
+    <mergeCell ref="B3:B19"/>
+    <mergeCell ref="C3:C19"/>
+    <mergeCell ref="F3:F15"/>
+    <mergeCell ref="G3:G15"/>
+    <mergeCell ref="H3:H17"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="B20:B28"/>
+    <mergeCell ref="C20:C28"/>
+    <mergeCell ref="E29:E43"/>
+    <mergeCell ref="E44:E54"/>
+    <mergeCell ref="F44:F51"/>
+    <mergeCell ref="G44:G51"/>
+    <mergeCell ref="H44:H54"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="E20:E25"/>
+    <mergeCell ref="F20:F25"/>
+    <mergeCell ref="F29:F40"/>
+    <mergeCell ref="G29:G40"/>
+    <mergeCell ref="H29:H40"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="G20:G25"/>
+    <mergeCell ref="H20:H25"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="A29:A43"/>
+    <mergeCell ref="B29:B43"/>
+    <mergeCell ref="C29:C43"/>
+    <mergeCell ref="B44:B54"/>
+    <mergeCell ref="C44:C54"/>
+    <mergeCell ref="F55:F62"/>
+    <mergeCell ref="F63:F65"/>
+    <mergeCell ref="H153:H155"/>
+    <mergeCell ref="H156:H158"/>
+    <mergeCell ref="G55:G62"/>
+    <mergeCell ref="H55:H62"/>
+    <mergeCell ref="H63:H65"/>
+    <mergeCell ref="H66:H68"/>
+    <mergeCell ref="F111:F113"/>
+    <mergeCell ref="F66:F68"/>
+    <mergeCell ref="F69:F81"/>
+    <mergeCell ref="G69:G81"/>
+    <mergeCell ref="F82:F84"/>
+    <mergeCell ref="G88:G110"/>
+    <mergeCell ref="F153:F155"/>
+    <mergeCell ref="F156:F158"/>
+    <mergeCell ref="B133:B158"/>
+    <mergeCell ref="C133:C158"/>
+    <mergeCell ref="E133:E158"/>
+    <mergeCell ref="H185:H207"/>
+    <mergeCell ref="H208:H210"/>
+    <mergeCell ref="H211:H233"/>
+    <mergeCell ref="H234:H236"/>
+    <mergeCell ref="H82:H84"/>
+    <mergeCell ref="H85:H87"/>
+    <mergeCell ref="H88:H110"/>
+    <mergeCell ref="H111:H113"/>
+    <mergeCell ref="H114:H129"/>
+    <mergeCell ref="H130:H132"/>
+    <mergeCell ref="H133:H152"/>
+    <mergeCell ref="E185:E210"/>
+    <mergeCell ref="F185:F207"/>
+    <mergeCell ref="G185:G207"/>
+    <mergeCell ref="F208:F210"/>
+    <mergeCell ref="A211:A236"/>
+    <mergeCell ref="B211:B236"/>
+    <mergeCell ref="C211:C236"/>
+    <mergeCell ref="E211:E236"/>
+    <mergeCell ref="F211:F233"/>
+    <mergeCell ref="G211:G233"/>
+    <mergeCell ref="F234:F236"/>
     <mergeCell ref="A159:A184"/>
     <mergeCell ref="B159:B184"/>
     <mergeCell ref="C159:C184"/>
@@ -4251,78 +4323,18 @@
     <mergeCell ref="B114:B132"/>
     <mergeCell ref="C114:C132"/>
     <mergeCell ref="A133:A158"/>
-    <mergeCell ref="E185:E210"/>
-    <mergeCell ref="F185:F207"/>
-    <mergeCell ref="G185:G207"/>
-    <mergeCell ref="F208:F210"/>
-    <mergeCell ref="A211:A236"/>
-    <mergeCell ref="B211:B236"/>
-    <mergeCell ref="C211:C236"/>
-    <mergeCell ref="E211:E236"/>
-    <mergeCell ref="F211:F233"/>
-    <mergeCell ref="G211:G233"/>
-    <mergeCell ref="F234:F236"/>
-    <mergeCell ref="H185:H207"/>
-    <mergeCell ref="H208:H210"/>
-    <mergeCell ref="H211:H233"/>
-    <mergeCell ref="H234:H236"/>
-    <mergeCell ref="H82:H84"/>
-    <mergeCell ref="H85:H87"/>
-    <mergeCell ref="H88:H110"/>
-    <mergeCell ref="H111:H113"/>
-    <mergeCell ref="H114:H129"/>
-    <mergeCell ref="H130:H132"/>
-    <mergeCell ref="H133:H152"/>
-    <mergeCell ref="A29:A43"/>
-    <mergeCell ref="B29:B43"/>
-    <mergeCell ref="C29:C43"/>
-    <mergeCell ref="B44:B54"/>
-    <mergeCell ref="C44:C54"/>
-    <mergeCell ref="F55:F62"/>
-    <mergeCell ref="F63:F65"/>
-    <mergeCell ref="H153:H155"/>
-    <mergeCell ref="H156:H158"/>
-    <mergeCell ref="G55:G62"/>
-    <mergeCell ref="H55:H62"/>
-    <mergeCell ref="H63:H65"/>
-    <mergeCell ref="H66:H68"/>
-    <mergeCell ref="F111:F113"/>
-    <mergeCell ref="F66:F68"/>
-    <mergeCell ref="F69:F81"/>
-    <mergeCell ref="G69:G81"/>
-    <mergeCell ref="F82:F84"/>
-    <mergeCell ref="G88:G110"/>
-    <mergeCell ref="F153:F155"/>
-    <mergeCell ref="F156:F158"/>
-    <mergeCell ref="B133:B158"/>
-    <mergeCell ref="C133:C158"/>
-    <mergeCell ref="E133:E158"/>
-    <mergeCell ref="E29:E43"/>
-    <mergeCell ref="E44:E54"/>
-    <mergeCell ref="F44:F51"/>
-    <mergeCell ref="G44:G51"/>
-    <mergeCell ref="H44:H54"/>
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="E20:E25"/>
-    <mergeCell ref="F20:F25"/>
-    <mergeCell ref="F29:F40"/>
-    <mergeCell ref="G29:G40"/>
-    <mergeCell ref="H29:H40"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="G20:G25"/>
-    <mergeCell ref="H20:H25"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="A3:A19"/>
-    <mergeCell ref="B3:B19"/>
-    <mergeCell ref="C3:C19"/>
-    <mergeCell ref="F3:F15"/>
-    <mergeCell ref="G3:G15"/>
-    <mergeCell ref="H3:H17"/>
-    <mergeCell ref="A20:A28"/>
-    <mergeCell ref="B20:B28"/>
-    <mergeCell ref="C20:C28"/>
+    <mergeCell ref="F159:F181"/>
+    <mergeCell ref="G159:G181"/>
+    <mergeCell ref="H159:H181"/>
+    <mergeCell ref="F182:F184"/>
+    <mergeCell ref="H182:H184"/>
+    <mergeCell ref="F85:F87"/>
+    <mergeCell ref="F88:F110"/>
+    <mergeCell ref="F114:F129"/>
+    <mergeCell ref="G114:G129"/>
+    <mergeCell ref="F130:F132"/>
+    <mergeCell ref="F133:F152"/>
+    <mergeCell ref="G133:G152"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>